<commit_message>
Subscription Management and Products
</commit_message>
<xml_diff>
--- a/TestData/Testdata.xlsx
+++ b/TestData/Testdata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="12060" windowHeight="6510"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="12060" windowHeight="6510" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Service" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Renewal Strategy" sheetId="4" r:id="rId4"/>
     <sheet name="Subscription Management" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -972,9 +972,6 @@
     <t>TRAILZ13</t>
   </si>
   <si>
-    <t>DOVETAIL SERVICES,800 GUILLAT AVENUE,KENT SCIENCE PARK,SITTINGBOURNE</t>
-  </si>
-  <si>
     <t>MENS RUNNING MAGAZINE</t>
   </si>
   <si>
@@ -994,13 +991,16 @@
   </si>
   <si>
     <t>DOVECU4533688</t>
+  </si>
+  <si>
+    <t>DOVETAIL SERVICES,800 GUILLAT AVENUE,KENT SCIENCE PARK,SITTINGBOURNE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1234,7 +1234,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1269,7 +1268,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1445,14 +1443,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AO139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
@@ -1484,7 +1482,7 @@
     <col min="31" max="31" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="17" t="s">
         <v>46</v>
       </c>
@@ -1510,7 +1508,7 @@
       <c r="U1" s="14"/>
       <c r="V1" s="14"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="14"/>
       <c r="B2" s="16" t="s">
         <v>3</v>
@@ -1561,7 +1559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="14"/>
       <c r="B3" s="18" t="s">
         <v>154</v>
@@ -1612,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="17" t="s">
         <v>50</v>
       </c>
@@ -1638,7 +1636,7 @@
       <c r="U4" s="14"/>
       <c r="V4" s="14"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22">
       <c r="A6" s="17" t="s">
         <v>47</v>
       </c>
@@ -1664,7 +1662,7 @@
       <c r="U6" s="14"/>
       <c r="V6" s="14"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22">
       <c r="A7" s="14"/>
       <c r="B7" s="16" t="s">
         <v>3</v>
@@ -1712,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="A8" s="14"/>
       <c r="B8" s="18" t="s">
         <v>154</v>
@@ -1760,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22">
       <c r="A9" s="17" t="s">
         <v>49</v>
       </c>
@@ -1786,7 +1784,7 @@
       <c r="U9" s="14"/>
       <c r="V9" s="14"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22">
       <c r="A11" s="17" t="s">
         <v>57</v>
       </c>
@@ -1812,7 +1810,7 @@
       <c r="U11" s="14"/>
       <c r="V11" s="14"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22">
       <c r="A12" s="14"/>
       <c r="B12" s="16" t="s">
         <v>3</v>
@@ -1878,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22">
       <c r="A13" s="14"/>
       <c r="B13" s="18" t="s">
         <v>154</v>
@@ -1944,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22">
       <c r="A14" s="17" t="s">
         <v>58</v>
       </c>
@@ -1970,7 +1968,7 @@
       <c r="U14" s="14"/>
       <c r="V14" s="14"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22">
       <c r="A16" s="17" t="s">
         <v>64</v>
       </c>
@@ -1996,7 +1994,7 @@
       <c r="U16" s="14"/>
       <c r="V16" s="14"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="14"/>
       <c r="B17" s="16" t="s">
         <v>3</v>
@@ -2047,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="14"/>
       <c r="B18" s="18" t="s">
         <v>154</v>
@@ -2059,7 +2057,7 @@
         <v>315</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>316</v>
@@ -2098,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -2124,7 +2122,7 @@
       <c r="U19" s="14"/>
       <c r="V19" s="14"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="17" t="s">
         <v>67</v>
       </c>
@@ -2150,7 +2148,7 @@
       <c r="U21" s="14"/>
       <c r="V21" s="14"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="14"/>
       <c r="B22" s="16" t="s">
         <v>3</v>
@@ -2201,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="14"/>
       <c r="B23" s="18" t="s">
         <v>154</v>
@@ -2252,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="17" t="s">
         <v>68</v>
       </c>
@@ -2278,7 +2276,7 @@
       <c r="U24" s="14"/>
       <c r="V24" s="14"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" s="17" t="s">
         <v>83</v>
       </c>
@@ -2304,7 +2302,7 @@
       <c r="U26" s="14"/>
       <c r="V26" s="14"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="14"/>
       <c r="B27" s="16" t="s">
         <v>3</v>
@@ -2370,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="14"/>
       <c r="B28" s="18" t="s">
         <v>154</v>
@@ -2436,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" s="17" t="s">
         <v>84</v>
       </c>
@@ -2462,7 +2460,7 @@
       <c r="U29" s="14"/>
       <c r="V29" s="14"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" s="17" t="s">
         <v>85</v>
       </c>
@@ -2488,7 +2486,7 @@
       <c r="U31" s="14"/>
       <c r="V31" s="14"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" s="14"/>
       <c r="B32" s="16" t="s">
         <v>3</v>
@@ -2527,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18">
       <c r="A33" s="14"/>
       <c r="B33" s="18" t="s">
         <v>154</v>
@@ -2566,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18">
       <c r="A34" s="17" t="s">
         <v>86</v>
       </c>
@@ -2588,7 +2586,7 @@
       <c r="Q34" s="14"/>
       <c r="R34" s="14"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18">
       <c r="A36" s="17" t="s">
         <v>88</v>
       </c>
@@ -2610,7 +2608,7 @@
       <c r="Q36" s="14"/>
       <c r="R36" s="14"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18">
       <c r="A37" s="14"/>
       <c r="B37" s="16" t="s">
         <v>3</v>
@@ -2658,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18">
       <c r="A38" s="14"/>
       <c r="B38" s="18" t="s">
         <v>154</v>
@@ -2706,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18">
       <c r="A39" s="17" t="s">
         <v>89</v>
       </c>
@@ -2728,7 +2726,7 @@
       <c r="Q39" s="14"/>
       <c r="R39" s="14"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18">
       <c r="A41" s="17" t="s">
         <v>96</v>
       </c>
@@ -2750,7 +2748,7 @@
       <c r="Q41" s="14"/>
       <c r="R41" s="14"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18">
       <c r="A42" s="14"/>
       <c r="B42" s="16" t="s">
         <v>3</v>
@@ -2777,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18">
       <c r="A43" s="14"/>
       <c r="B43" s="18" t="s">
         <v>154</v>
@@ -2804,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18">
       <c r="A44" s="17" t="s">
         <v>97</v>
       </c>
@@ -2826,7 +2824,7 @@
       <c r="Q44" s="14"/>
       <c r="R44" s="14"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18">
       <c r="A46" s="17" t="s">
         <v>108</v>
       </c>
@@ -2848,7 +2846,7 @@
       <c r="Q46" s="14"/>
       <c r="R46" s="14"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18">
       <c r="A47" s="14"/>
       <c r="B47" s="16" t="s">
         <v>3</v>
@@ -2902,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18">
       <c r="A48" s="14"/>
       <c r="B48" s="18" t="s">
         <v>154</v>
@@ -2917,7 +2915,7 @@
         <v>158</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>155</v>
@@ -2956,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19">
       <c r="A49" s="17" t="s">
         <v>109</v>
       </c>
@@ -2979,7 +2977,7 @@
       <c r="R49" s="14"/>
       <c r="S49" s="14"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19">
       <c r="A51" s="17" t="s">
         <v>112</v>
       </c>
@@ -3002,7 +3000,7 @@
       <c r="R51" s="14"/>
       <c r="S51" s="14"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19">
       <c r="A52" s="14"/>
       <c r="B52" s="16" t="s">
         <v>3</v>
@@ -3059,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19">
       <c r="A53" s="14"/>
       <c r="B53" s="18" t="s">
         <v>154</v>
@@ -3116,7 +3114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19">
       <c r="A54" s="17" t="s">
         <v>113</v>
       </c>
@@ -3139,7 +3137,7 @@
       <c r="R54" s="14"/>
       <c r="S54" s="14"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19">
       <c r="A56" s="17" t="s">
         <v>114</v>
       </c>
@@ -3162,7 +3160,7 @@
       <c r="R56" s="14"/>
       <c r="S56" s="14"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19">
       <c r="A57" s="14"/>
       <c r="B57" s="16" t="s">
         <v>3</v>
@@ -3186,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19">
       <c r="A58" s="14"/>
       <c r="B58" s="18" t="s">
         <v>154</v>
@@ -3210,7 +3208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19">
       <c r="A59" s="17" t="s">
         <v>115</v>
       </c>
@@ -3233,7 +3231,7 @@
       <c r="R59" s="14"/>
       <c r="S59" s="14"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19">
       <c r="A61" s="17" t="s">
         <v>118</v>
       </c>
@@ -3256,7 +3254,7 @@
       <c r="R61" s="14"/>
       <c r="S61" s="14"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19">
       <c r="A62" s="14"/>
       <c r="B62" s="16" t="s">
         <v>3</v>
@@ -3280,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19">
       <c r="A63" s="14"/>
       <c r="B63" s="18" t="s">
         <v>154</v>
@@ -3304,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19">
       <c r="A64" s="17" t="s">
         <v>119</v>
       </c>
@@ -3327,7 +3325,7 @@
       <c r="R64" s="14"/>
       <c r="S64" s="14"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19">
       <c r="A66" s="17" t="s">
         <v>122</v>
       </c>
@@ -3350,7 +3348,7 @@
       <c r="R66" s="14"/>
       <c r="S66" s="14"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19">
       <c r="A67" s="14"/>
       <c r="B67" s="16" t="s">
         <v>3</v>
@@ -3377,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19">
       <c r="A68" s="14"/>
       <c r="B68" s="18" t="s">
         <v>154</v>
@@ -3404,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19">
       <c r="A69" s="17" t="s">
         <v>123</v>
       </c>
@@ -3427,7 +3425,7 @@
       <c r="R69" s="14"/>
       <c r="S69" s="14"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19">
       <c r="A71" s="17" t="s">
         <v>127</v>
       </c>
@@ -3450,7 +3448,7 @@
       <c r="R71" s="14"/>
       <c r="S71" s="14"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19">
       <c r="A72" s="14"/>
       <c r="B72" s="16" t="s">
         <v>3</v>
@@ -3507,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19">
       <c r="A73" s="14"/>
       <c r="B73" s="18" t="s">
         <v>154</v>
@@ -3534,7 +3532,7 @@
         <v>149</v>
       </c>
       <c r="J73" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K73" s="15" t="s">
         <v>150</v>
@@ -3558,7 +3556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19">
       <c r="A74" s="17" t="s">
         <v>128</v>
       </c>
@@ -3581,7 +3579,7 @@
       <c r="R74" s="14"/>
       <c r="S74" s="14"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19">
       <c r="A76" s="17" t="s">
         <v>134</v>
       </c>
@@ -3604,7 +3602,7 @@
       <c r="R76" s="14"/>
       <c r="S76" s="14"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19">
       <c r="A77" s="14"/>
       <c r="B77" s="16" t="s">
         <v>3</v>
@@ -3628,7 +3626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19">
       <c r="A78" s="14"/>
       <c r="B78" s="18" t="s">
         <v>154</v>
@@ -3652,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19">
       <c r="A79" s="17" t="s">
         <v>135</v>
       </c>
@@ -3675,7 +3673,7 @@
       <c r="R79" s="14"/>
       <c r="S79" s="14"/>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:41">
       <c r="A81" s="17" t="s">
         <v>140</v>
       </c>
@@ -3720,7 +3718,7 @@
       <c r="AN81" s="14"/>
       <c r="AO81" s="14"/>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:41">
       <c r="A82" s="14"/>
       <c r="B82" s="16" t="s">
         <v>3</v>
@@ -3753,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:41">
       <c r="A83" s="14"/>
       <c r="B83" s="18" t="s">
         <v>154</v>
@@ -3786,7 +3784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:41">
       <c r="A84" s="17" t="s">
         <v>141</v>
       </c>
@@ -3831,7 +3829,7 @@
       <c r="AN84" s="14"/>
       <c r="AO84" s="14"/>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:41">
       <c r="A86" s="17" t="s">
         <v>238</v>
       </c>
@@ -3876,7 +3874,7 @@
       <c r="AN86" s="14"/>
       <c r="AO86" s="14"/>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:41">
       <c r="A87" s="14"/>
       <c r="B87" s="16" t="s">
         <v>3</v>
@@ -3918,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:41">
       <c r="A88" s="14"/>
       <c r="B88" s="18" t="s">
         <v>154</v>
@@ -3960,7 +3958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:41">
       <c r="A89" s="17" t="s">
         <v>243</v>
       </c>
@@ -4005,7 +4003,7 @@
       <c r="AN89" s="14"/>
       <c r="AO89" s="14"/>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:41">
       <c r="A91" s="17" t="s">
         <v>244</v>
       </c>
@@ -4050,7 +4048,7 @@
       <c r="AN91" s="14"/>
       <c r="AO91" s="14"/>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:41">
       <c r="A92" s="14"/>
       <c r="B92" s="16" t="s">
         <v>3</v>
@@ -4083,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:41">
       <c r="A93" s="14"/>
       <c r="B93" s="18" t="s">
         <v>154</v>
@@ -4116,7 +4114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:41">
       <c r="A94" s="17" t="s">
         <v>247</v>
       </c>
@@ -4161,7 +4159,7 @@
       <c r="AN94" s="14"/>
       <c r="AO94" s="14"/>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:41">
       <c r="A95" s="14"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
@@ -4204,7 +4202,7 @@
       <c r="AN95" s="14"/>
       <c r="AO95" s="14"/>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:41">
       <c r="A96" s="17" t="s">
         <v>248</v>
       </c>
@@ -4249,7 +4247,7 @@
       <c r="AN96" s="14"/>
       <c r="AO96" s="14"/>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:41">
       <c r="A97" s="14"/>
       <c r="B97" s="16" t="s">
         <v>3</v>
@@ -4273,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:41">
       <c r="A98" s="14"/>
       <c r="B98" s="18" t="s">
         <v>154</v>
@@ -4297,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:41">
       <c r="A99" s="17" t="s">
         <v>251</v>
       </c>
@@ -4342,7 +4340,7 @@
       <c r="AN99" s="14"/>
       <c r="AO99" s="14"/>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:41">
       <c r="A100" s="14"/>
       <c r="B100" s="14"/>
       <c r="C100" s="14"/>
@@ -4385,7 +4383,7 @@
       <c r="AN100" s="14"/>
       <c r="AO100" s="14"/>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:41">
       <c r="A101" s="17" t="s">
         <v>252</v>
       </c>
@@ -4430,7 +4428,7 @@
       <c r="AN101" s="14"/>
       <c r="AO101" s="14"/>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:41">
       <c r="A102" s="14"/>
       <c r="B102" s="16" t="s">
         <v>3</v>
@@ -4487,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:41">
       <c r="A103" s="14"/>
       <c r="B103" s="18" t="s">
         <v>154</v>
@@ -4544,7 +4542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:41">
       <c r="A104" s="17" t="s">
         <v>257</v>
       </c>
@@ -4589,7 +4587,7 @@
       <c r="AN104" s="14"/>
       <c r="AO104" s="14"/>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:41">
       <c r="A105" s="14"/>
       <c r="B105" s="14"/>
       <c r="C105" s="14"/>
@@ -4632,7 +4630,7 @@
       <c r="AN105" s="14"/>
       <c r="AO105" s="14"/>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:41">
       <c r="A106" s="17" t="s">
         <v>258</v>
       </c>
@@ -4677,7 +4675,7 @@
       <c r="AN106" s="14"/>
       <c r="AO106" s="14"/>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:41">
       <c r="A107" s="14"/>
       <c r="B107" s="14"/>
       <c r="C107" s="14"/>
@@ -4720,7 +4718,7 @@
       <c r="AN107" s="14"/>
       <c r="AO107" s="14"/>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:41">
       <c r="A108" s="14"/>
       <c r="B108" s="14"/>
       <c r="C108" s="14"/>
@@ -4763,7 +4761,7 @@
       <c r="AN108" s="14"/>
       <c r="AO108" s="14"/>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:41">
       <c r="A109" s="17" t="s">
         <v>259</v>
       </c>
@@ -4808,7 +4806,7 @@
       <c r="AN109" s="14"/>
       <c r="AO109" s="14"/>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:41">
       <c r="A110" s="14"/>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
@@ -4851,7 +4849,7 @@
       <c r="AN110" s="14"/>
       <c r="AO110" s="14"/>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:41">
       <c r="A111" s="17" t="s">
         <v>260</v>
       </c>
@@ -4896,7 +4894,7 @@
       <c r="AN111" s="14"/>
       <c r="AO111" s="14"/>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:41">
       <c r="A112" s="14"/>
       <c r="B112" s="16" t="s">
         <v>3</v>
@@ -4923,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:41">
       <c r="A113" s="14"/>
       <c r="B113" s="18" t="s">
         <v>154</v>
@@ -4950,7 +4948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:41">
       <c r="A114" s="17" t="s">
         <v>263</v>
       </c>
@@ -4995,7 +4993,7 @@
       <c r="AN114" s="14"/>
       <c r="AO114" s="14"/>
     </row>
-    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:41">
       <c r="A115" s="14"/>
       <c r="B115" s="14"/>
       <c r="C115" s="14"/>
@@ -5038,7 +5036,7 @@
       <c r="AN115" s="14"/>
       <c r="AO115" s="14"/>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:41">
       <c r="A116" s="17" t="s">
         <v>264</v>
       </c>
@@ -5083,7 +5081,7 @@
       <c r="AN116" s="14"/>
       <c r="AO116" s="14"/>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:41">
       <c r="A117" s="14"/>
       <c r="B117" s="16" t="s">
         <v>3</v>
@@ -5107,7 +5105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:41">
       <c r="A118" s="14"/>
       <c r="B118" s="18" t="s">
         <v>154</v>
@@ -5131,7 +5129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:41">
       <c r="A119" s="17" t="s">
         <v>265</v>
       </c>
@@ -5176,7 +5174,7 @@
       <c r="AN119" s="14"/>
       <c r="AO119" s="14"/>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:41">
       <c r="A121" s="17" t="s">
         <v>266</v>
       </c>
@@ -5221,7 +5219,7 @@
       <c r="AN121" s="14"/>
       <c r="AO121" s="14"/>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:41">
       <c r="A122" s="14"/>
       <c r="B122" s="16" t="s">
         <v>3</v>
@@ -5272,7 +5270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:41">
       <c r="A123" s="14"/>
       <c r="B123" s="18" t="s">
         <v>154</v>
@@ -5299,7 +5297,7 @@
         <v>224</v>
       </c>
       <c r="J123" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K123" s="15" t="s">
         <v>15</v>
@@ -5323,7 +5321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:41">
       <c r="A124" s="17" t="s">
         <v>270</v>
       </c>
@@ -5368,7 +5366,7 @@
       <c r="AN124" s="14"/>
       <c r="AO124" s="14"/>
     </row>
-    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:41">
       <c r="A126" s="17" t="s">
         <v>271</v>
       </c>
@@ -5413,7 +5411,7 @@
       <c r="AN126" s="14"/>
       <c r="AO126" s="14"/>
     </row>
-    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:41">
       <c r="A127" s="14"/>
       <c r="B127" s="16" t="s">
         <v>3</v>
@@ -5506,7 +5504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:41">
       <c r="A128" s="14"/>
       <c r="B128" s="18" t="s">
         <v>154</v>
@@ -5533,7 +5531,7 @@
         <v>224</v>
       </c>
       <c r="J128" s="15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K128" s="15" t="s">
         <v>15</v>
@@ -5599,7 +5597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20">
       <c r="A129" s="17" t="s">
         <v>284</v>
       </c>
@@ -5623,7 +5621,7 @@
       <c r="S129" s="14"/>
       <c r="T129" s="14"/>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20">
       <c r="A131" s="17" t="s">
         <v>285</v>
       </c>
@@ -5647,7 +5645,7 @@
       <c r="S131" s="14"/>
       <c r="T131" s="14"/>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20">
       <c r="A132" s="14"/>
       <c r="B132" s="16" t="s">
         <v>3</v>
@@ -5707,7 +5705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20">
       <c r="A133" s="14"/>
       <c r="B133" s="18" t="s">
         <v>154</v>
@@ -5734,7 +5732,7 @@
         <v>224</v>
       </c>
       <c r="J133" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K133" s="15" t="s">
         <v>15</v>
@@ -5767,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20">
       <c r="A134" s="17" t="s">
         <v>292</v>
       </c>
@@ -5791,7 +5789,7 @@
       <c r="S134" s="14"/>
       <c r="T134" s="14"/>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20">
       <c r="A136" s="17" t="s">
         <v>293</v>
       </c>
@@ -5815,7 +5813,7 @@
       <c r="S136" s="14"/>
       <c r="T136" s="14"/>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20">
       <c r="A137" s="14"/>
       <c r="B137" s="16" t="s">
         <v>3</v>
@@ -5836,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20">
       <c r="A138" s="14"/>
       <c r="B138" s="18" t="s">
         <v>154</v>
@@ -5857,7 +5855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20">
       <c r="A139" s="17" t="s">
         <v>294</v>
       </c>
@@ -5918,14 +5916,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -5935,12 +5933,12 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -5954,7 +5952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="B3" s="5" t="s">
         <v>82</v>
       </c>
@@ -5968,7 +5966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>93</v>
       </c>
@@ -5982,14 +5980,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -6010,12 +6008,12 @@
     <col min="17" max="17" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -6059,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="B3" s="5" t="s">
         <v>82</v>
       </c>
@@ -6103,17 +6101,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -6157,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="B8" s="5" t="s">
         <v>82</v>
       </c>
@@ -6201,17 +6199,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -6261,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="B13" s="5" t="s">
         <v>82</v>
       </c>
@@ -6311,17 +6309,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
@@ -6377,7 +6375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="B18" s="5" t="s">
         <v>82</v>
       </c>
@@ -6433,17 +6431,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="B22" s="2" t="s">
         <v>3</v>
       </c>
@@ -6469,7 +6467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="B23" s="5" t="s">
         <v>82</v>
       </c>
@@ -6495,17 +6493,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="4" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
@@ -6549,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="B28" s="5" t="s">
         <v>82</v>
       </c>
@@ -6593,7 +6591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="4" t="s">
         <v>185</v>
       </c>
@@ -6611,14 +6609,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -6637,12 +6635,12 @@
     <col min="17" max="17" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -6686,7 +6684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="B3" s="5" t="s">
         <v>82</v>
       </c>
@@ -6730,17 +6728,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
@@ -6796,7 +6794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="B8" s="5" t="s">
         <v>82</v>
       </c>
@@ -6852,17 +6850,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
@@ -6918,7 +6916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="B13" s="5" t="s">
         <v>82</v>
       </c>
@@ -6974,17 +6972,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
@@ -7040,7 +7038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="B18" s="5" t="s">
         <v>82</v>
       </c>
@@ -7096,12 +7094,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="127" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="11:11">
       <c r="K127" t="s">
         <v>197</v>
       </c>
@@ -7119,14 +7117,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.140625" style="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="27" bestFit="1" customWidth="1"/>
@@ -7140,7 +7138,7 @@
     <col min="10" max="10" width="17.7109375" style="27" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="10.140625" style="27" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="30" style="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" style="27" customWidth="1"/>
     <col min="16" max="16" width="30" style="27" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.28515625" style="27" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="27" bestFit="1" customWidth="1"/>
@@ -7152,12 +7150,12 @@
     <col min="26" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25">
       <c r="A1" s="26" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25">
       <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
@@ -7231,7 +7229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="45">
       <c r="B3" s="18" t="s">
         <v>154</v>
       </c>
@@ -7266,10 +7264,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="O3" s="29" t="s">
         <v>156</v>
@@ -7305,17 +7303,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25">
       <c r="A4" s="26" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25">
       <c r="A6" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25">
       <c r="B7" s="28" t="s">
         <v>3</v>
       </c>
@@ -7383,7 +7381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="105">
       <c r="B8" s="18" t="s">
         <v>154</v>
       </c>
@@ -7409,7 +7407,7 @@
         <v>297</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K8" s="29" t="s">
         <v>17</v>
@@ -7421,10 +7419,10 @@
         <v>16</v>
       </c>
       <c r="N8" s="29" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="P8" s="29" t="s">
         <v>156</v>
@@ -7451,17 +7449,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25">
       <c r="A9" s="26" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25">
       <c r="A11" s="26" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25">
       <c r="B12" s="28" t="s">
         <v>3</v>
       </c>
@@ -7529,7 +7527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="45">
       <c r="B13" s="18" t="s">
         <v>154</v>
       </c>
@@ -7540,7 +7538,7 @@
         <v>315</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>161</v>
@@ -7555,7 +7553,7 @@
         <v>297</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K13" s="33">
         <v>2</v>
@@ -7570,10 +7568,10 @@
         <v>16</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
       <c r="P13" s="31" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="Q13" s="11" t="s">
         <v>23</v>
@@ -7597,12 +7595,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25">
       <c r="A14" s="26" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5">
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>

</xml_diff>